<commit_message>
added text explantion of results
</commit_message>
<xml_diff>
--- a/Program1/Results.xlsx
+++ b/Program1/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCodeWorkspace\CSI_3344\Program1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DFE8CCC-D1CC-41A0-AFBD-7CF146B929D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9D3053-D0C0-4DF8-A296-722EC99B4B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-6550" windowWidth="38620" windowHeight="21820" xr2:uid="{C031439D-1BB6-4FB5-8493-EE10A076EA35}"/>
   </bookViews>
@@ -1270,6 +1270,90 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257969</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>591343</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>91281</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E9ECEB4-571E-706A-63BD-57F514535C24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257969" y="3929063"/>
+          <a:ext cx="11707812" cy="2067718"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Based on the results above, It</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> seems that(at least with this implementation of quicksort) using the median of three is generally the better approach. However, no only does this not take into account the comparisons to find the median, but random had very similar performance, outperforming Median of three slightly on the semi sorted 2k and the 10k tests. This does not make random the better method though, since as the name implies it is random. It is possible for random to chose the first or last point as the pivot which would reslut in signifigantly worse performace for any slightly sorted data set. Median of three seems to be consistently good at choosing a good pivot value. In regards to the first and final pivot values, first actually performed slightly better for the completley unsorted data set, but it performed signifigantly worse for every other test, with it performing the maximum possible number of comparisons for the reverse values. An interesting subject is the final pivot value. One would expect the results from this to be similar to choosing the first value, but for every test it performed the maxium number of comparisons. As far as I can tell, this is something unique to this specifc implementation of quicksort, as testing different implementations resulted in better performance. I belive this is because for this implementation if the pivot value is the final one, then the algorithim will only partition one off the end every time resulting in the horrible performance we have here.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>To conclude, with this implementation Median of three had the best performance, but judging by these limited tests, if the data is expected to be sorted or mostly sorted, than chosing a random pivot value would be better. (Or a different sorting algorithim)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1573,7 +1657,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>